<commit_message>
creation de la concepmap valueset et codesystem
creation de la concepmap valueset et codesystem 3e3120987b0da7687bb02892f3058c35e1f17481
</commit_message>
<xml_diff>
--- a/ig/sd-phase-de-lessai-creation-conceptmap/CodeSystem-eclaire-study-phase-code-system.xlsx
+++ b/ig/sd-phase-de-lessai-creation-conceptmap/CodeSystem-eclaire-study-phase-code-system.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-08-30T08:25:30+00:00</t>
+    <t>2023-08-30T14:09:22+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>Phase III and phase IV (Integrated)</t>
+  </si>
+  <si>
+    <t>Trials that are a combination of phases III and IV.</t>
   </si>
 </sst>
 </file>
@@ -460,7 +463,9 @@
       <c r="C2" t="s" s="2">
         <v>38</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" t="s" s="2">
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>